<commit_message>
Add selector for appender service
</commit_message>
<xml_diff>
--- a/docs/PerformanceGenerator.xlsx
+++ b/docs/PerformanceGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaronprigal/sources/github/sample-azure-eventer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF1264D-529F-2140-AD24-EB20C47814B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E54711-E76C-CE42-85C7-AB020429CBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7CFC8003-B321-4E4E-99AF-FD7AA9F6F2E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="96">
   <si>
     <t>300ms</t>
   </si>
@@ -775,6 +775,123 @@
       </rPr>
       <t xml:space="preserve"> /
 00:00:00.967</t>
+    </r>
+  </si>
+  <si>
+    <t>950ms</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00:00:17.649</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>00:00:17.421</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">+
+00:00:00.248 /
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00:00:35.959</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>00:00:35.742</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /
+00:00:00.317</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>200 files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>per sec 
+/per process (appender service run across 3 nodes f4s_v2)</t>
     </r>
   </si>
 </sst>
@@ -1556,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B43E74-5CC3-EB49-A9D0-22415A944AAB}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="247" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,14 +1686,14 @@
     <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="7" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>63</v>
       </c>
@@ -1590,8 +1707,9 @@
       <c r="G1" s="62"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
-    </row>
-    <row r="2" spans="1:11" ht="44" x14ac:dyDescent="0.2">
+      <c r="J1" s="62"/>
+    </row>
+    <row r="2" spans="1:12" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="66" t="s">
         <v>85</v>
       </c>
@@ -1612,13 +1730,16 @@
         <v>67</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="18"/>
@@ -1637,15 +1758,19 @@
         <v>200</v>
       </c>
       <c r="H3" s="34">
+        <f>D3*200</f>
+        <v>200</v>
+      </c>
+      <c r="I3" s="34">
         <f>D3*300</f>
         <v>300</v>
       </c>
-      <c r="I3" s="34">
+      <c r="J3" s="34">
         <f>D3*500</f>
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
         <v>91</v>
@@ -1657,19 +1782,22 @@
         <v>54</v>
       </c>
       <c r="G4" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="J4" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="63" t="s">
+      <c r="L4" s="63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="67"/>
       <c r="B5" s="73" t="s">
         <v>86</v>
@@ -1681,11 +1809,14 @@
       <c r="G5" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="72"/>
-      <c r="K5" s="63"/>
-    </row>
-    <row r="6" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="H5" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
+      <c r="L5" s="63"/>
+    </row>
+    <row r="6" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="67"/>
       <c r="B6" s="73" t="s">
         <v>90</v>
@@ -1697,11 +1828,14 @@
       <c r="G6" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="71"/>
-      <c r="I6" s="72"/>
-      <c r="K6" s="64"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="L6" s="64"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="28" t="s">
         <v>74</v>
@@ -1719,11 +1853,14 @@
         <v>36</v>
       </c>
       <c r="I7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="64"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="64"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="28" t="s">
         <v>75</v>
@@ -1738,14 +1875,17 @@
         <v>14</v>
       </c>
       <c r="H8" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="J8" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="64"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="64"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="29" t="s">
         <v>7</v>
@@ -1757,17 +1897,20 @@
         <v>0.16</v>
       </c>
       <c r="G9" s="53">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="H9" s="53">
+        <v>0.33</v>
+      </c>
+      <c r="I9" s="53">
         <v>0.46</v>
       </c>
-      <c r="I9" s="53">
+      <c r="J9" s="53">
         <v>0.43</v>
       </c>
-      <c r="K9" s="64"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="64"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1782,20 +1925,24 @@
         <v>200</v>
       </c>
       <c r="G10" s="20">
+        <f>C10*200</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
         <f>D10*200</f>
         <v>400</v>
       </c>
-      <c r="H10" s="20">
+      <c r="I10" s="20">
         <f>D10*300</f>
         <v>600</v>
       </c>
-      <c r="I10" s="20">
+      <c r="J10" s="20">
         <f>D10*500</f>
         <v>1000</v>
       </c>
-      <c r="K10" s="64"/>
-    </row>
-    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L10" s="64"/>
+    </row>
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="38" t="s">
         <v>1</v>
@@ -1812,14 +1959,17 @@
         <v>50</v>
       </c>
       <c r="H11" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="57" t="s">
+      <c r="J11" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="64"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="64"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="39" t="s">
         <v>74</v>
@@ -1834,14 +1984,17 @@
         <v>51</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="I12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="64"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="64"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="39" t="s">
         <v>75</v>
@@ -1856,14 +2009,17 @@
         <v>31</v>
       </c>
       <c r="H13" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="55" t="s">
+      <c r="J13" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="64"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="64"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="37"/>
       <c r="B14" s="40" t="s">
         <v>7</v>
@@ -1878,14 +2034,17 @@
         <v>0.42</v>
       </c>
       <c r="H14" s="56">
+        <v>0.42</v>
+      </c>
+      <c r="I14" s="56">
         <v>0.94</v>
       </c>
-      <c r="I14" s="56">
+      <c r="J14" s="56">
         <v>0.95</v>
       </c>
-      <c r="K14" s="64"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="64"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1900,20 +2059,24 @@
         <v>300</v>
       </c>
       <c r="G15" s="20">
+        <f>C15*200</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
         <f>D15*200</f>
         <v>600</v>
       </c>
-      <c r="H15" s="20">
+      <c r="I15" s="20">
         <f>D15*300</f>
         <v>900</v>
       </c>
-      <c r="I15" s="20">
+      <c r="J15" s="20">
         <f>D15*500</f>
         <v>1500</v>
       </c>
-      <c r="K15" s="65"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="65"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
       <c r="B16" s="43" t="s">
         <v>1</v>
@@ -1928,14 +2091,17 @@
         <v>23</v>
       </c>
       <c r="H16" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="J16" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="65"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="65"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
       <c r="B17" s="44" t="s">
         <v>74</v>
@@ -1955,9 +2121,12 @@
       <c r="I17" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="65"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J17" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="65"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
       <c r="B18" s="44" t="s">
         <v>75</v>
@@ -1972,14 +2141,17 @@
         <v>47</v>
       </c>
       <c r="H18" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="J18" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="65"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="65"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
       <c r="B19" s="45" t="s">
         <v>11</v>
@@ -1994,14 +2166,17 @@
         <v>0.87</v>
       </c>
       <c r="H19" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="I19" s="53">
         <v>0.95</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="J19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="65"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="65"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
@@ -2009,9 +2184,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="K20" s="65"/>
-    </row>
-    <row r="21" spans="1:11" ht="44" x14ac:dyDescent="0.2">
+      <c r="J20" s="2"/>
+      <c r="L20" s="65"/>
+    </row>
+    <row r="21" spans="1:12" ht="44" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>64</v>
       </c>
@@ -2032,14 +2208,17 @@
         <v>67</v>
       </c>
       <c r="H21" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="J21" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="65"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="65"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="18"/>
@@ -2054,19 +2233,23 @@
         <v>100</v>
       </c>
       <c r="G22" s="34">
+        <f>C22*200</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="34">
         <f>D22*200</f>
         <v>200</v>
       </c>
-      <c r="H22" s="34">
+      <c r="I22" s="34">
         <f>D22*300</f>
         <v>300</v>
       </c>
-      <c r="I22" s="34">
+      <c r="J22" s="34">
         <f>D22*500</f>
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="38" t="s">
         <v>1</v>
@@ -2080,14 +2263,17 @@
       <c r="G23" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="57" t="s">
+      <c r="H23" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="57" t="s">
+      <c r="J23" s="57" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="39" t="s">
         <v>74</v>
@@ -2107,8 +2293,11 @@
       <c r="I24" s="50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J24" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="36"/>
       <c r="B25" s="39" t="s">
         <v>75</v>
@@ -2123,13 +2312,16 @@
         <v>14</v>
       </c>
       <c r="H25" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="50" t="s">
+      <c r="J25" s="50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="36"/>
       <c r="B26" s="40" t="s">
         <v>11</v>
@@ -2144,13 +2336,16 @@
         <v>0.3</v>
       </c>
       <c r="H26" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="I26" s="51">
         <v>0.33</v>
       </c>
-      <c r="I26" s="51">
+      <c r="J26" s="51">
         <v>0.52</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2165,19 +2360,23 @@
         <v>200</v>
       </c>
       <c r="G27" s="20">
+        <f>C27*200</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="20">
         <f>D27*200</f>
         <v>400</v>
       </c>
-      <c r="H27" s="20">
+      <c r="I27" s="20">
         <f>D27*300</f>
         <v>600</v>
       </c>
-      <c r="I27" s="20">
+      <c r="J27" s="20">
         <f>D27*500</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>1</v>
@@ -2191,14 +2390,17 @@
       <c r="G28" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="59" t="s">
+      <c r="J28" s="59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
       <c r="B29" s="10" t="s">
         <v>74</v>
@@ -2212,14 +2414,17 @@
       <c r="G29" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="47" t="s">
+      <c r="J29" s="47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
       <c r="B30" s="10" t="s">
         <v>75</v>
@@ -2233,14 +2438,17 @@
       <c r="G30" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I30" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J30" s="47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>11</v>
@@ -2254,14 +2462,17 @@
       <c r="G31" s="53">
         <v>0.48</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="53">
+        <v>0.48</v>
+      </c>
+      <c r="I31" s="13">
         <v>0.74</v>
       </c>
-      <c r="I31" s="53">
+      <c r="J31" s="53">
         <v>0.95</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -2276,19 +2487,23 @@
         <v>300</v>
       </c>
       <c r="G32" s="20">
+        <f>C32*200</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="20">
         <f>D32*200</f>
         <v>600</v>
       </c>
-      <c r="H32" s="20">
+      <c r="I32" s="20">
         <f>D32*300</f>
         <v>900</v>
       </c>
-      <c r="I32" s="20">
+      <c r="J32" s="20">
         <f>D32*500</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="35"/>
       <c r="B33" s="38" t="s">
         <v>1</v>
@@ -2303,13 +2518,16 @@
         <v>23</v>
       </c>
       <c r="H33" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="57" t="s">
+      <c r="J33" s="57" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="36"/>
       <c r="B34" s="39" t="s">
         <v>74</v>
@@ -2327,10 +2545,13 @@
         <v>26</v>
       </c>
       <c r="I34" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="36"/>
       <c r="B35" s="39" t="s">
         <v>75</v>
@@ -2345,13 +2566,16 @@
         <v>24</v>
       </c>
       <c r="H35" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="50" t="s">
+      <c r="J35" s="50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="37"/>
       <c r="B36" s="40" t="s">
         <v>11</v>
@@ -2366,14 +2590,17 @@
         <v>0.65</v>
       </c>
       <c r="H36" s="51">
+        <v>0.65</v>
+      </c>
+      <c r="I36" s="51">
         <v>0.73</v>
       </c>
-      <c r="I36" s="51">
+      <c r="J36" s="51">
         <v>0.95</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>6</v>
       </c>
@@ -2394,13 +2621,16 @@
         <v>58</v>
       </c>
       <c r="H38" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="I38" s="60" t="s">
+      <c r="J38" s="60" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="5" t="s">
         <v>1</v>
@@ -2417,15 +2647,18 @@
         <v>3</v>
       </c>
       <c r="H39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="J39" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K4:K21"/>
+    <mergeCell ref="L4:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update checkpoint in case of exception
</commit_message>
<xml_diff>
--- a/docs/PerformanceGenerator.xlsx
+++ b/docs/PerformanceGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaronprigal/sources/github/sample-azure-eventer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C30C5D-030C-9240-890A-008F427613E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1A111F-D343-D74D-AEB3-02BB3CD4FC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7CFC8003-B321-4E4E-99AF-FD7AA9F6F2E9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7CFC8003-B321-4E4E-99AF-FD7AA9F6F2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3936,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B43E74-5CC3-EB49-A9D0-22415A944AAB}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="116" zoomScaleNormal="247" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5455,8 +5455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385BE553-DAEA-2B4A-9C29-7E81AC3CC68B}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B34" sqref="A30:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>